<commit_message>
Can Load files of synthetic population
Also description of citizens and families has been added
</commit_message>
<xml_diff>
--- a/Archetypes/citizen_archetypes.xlsx
+++ b/Archetypes/citizen_archetypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\Archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251DFA97-518C-422A-B7C2-C9F8825F600F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB81DD6-95C4-4F3E-A10B-7F54858EA135}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E19" sqref="D11:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
archetypes excel has changed
</commit_message>
<xml_diff>
--- a/Archetypes/citizen_archetypes.xlsx
+++ b/Archetypes/citizen_archetypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\Archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C82D96F-002E-4531-A989-3964CCECCC21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345EF54F-1B3B-4FB7-9B58-F18AAB231F8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -42,18 +42,6 @@
     <t>active</t>
   </si>
   <si>
-    <t>dependency</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>WoS_state</t>
-  </si>
-  <si>
     <t>work</t>
   </si>
   <si>
@@ -63,21 +51,6 @@
     <t>study</t>
   </si>
   <si>
-    <t>family_types</t>
-  </si>
-  <si>
-    <t>h,f,w</t>
-  </si>
-  <si>
-    <t>h,s</t>
-  </si>
-  <si>
-    <t>h,*</t>
-  </si>
-  <si>
-    <t>h,f</t>
-  </si>
-  <si>
     <t>c_arch_0</t>
   </si>
   <si>
@@ -106,18 +79,30 @@
   </si>
   <si>
     <t>youth</t>
+  </si>
+  <si>
+    <t>WoS_type</t>
+  </si>
+  <si>
+    <t>WoS_mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -141,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,23 +409,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,21 +441,18 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>57</v>
@@ -476,21 +461,18 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>57</v>
@@ -499,21 +481,18 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>80</v>
@@ -524,19 +503,16 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -545,18 +521,18 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>18</v>
@@ -567,12 +543,25 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>